<commit_message>
Product Backlog file Revised
</commit_message>
<xml_diff>
--- a/Project/SMU 5510 Product Backlog.xlsx
+++ b/Project/SMU 5510 Product Backlog.xlsx
@@ -5,19 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nawazhussain/Desktop/Project 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nawazhussain/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D3F04D-F057-C747-B349-130CB754F63E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA84013-3546-4C40-9F2A-30B2A52522B5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog - Meeting 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog 1" sheetId="2" r:id="rId2"/>
     <sheet name="Product Backlog - Meeting 2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint Backlog 2" sheetId="4" r:id="rId4"/>
-    <sheet name="Team Members" sheetId="7" r:id="rId5"/>
+    <sheet name="Sprint Backlog 3 - Meeting 3" sheetId="8" r:id="rId5"/>
+    <sheet name="Sprint Backlog 3" sheetId="9" r:id="rId6"/>
+    <sheet name="Team Members" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -37,7 +39,7 @@
     <author>Dan Penny</author>
   </authors>
   <commentList>
-    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -117,8 +119,51 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dan Penny</author>
+  </authors>
+  <commentList>
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{3A483525-C7BA-104C-9B9D-12C5E319EA2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dan Penny:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Update Bus Value and Effort and ROI for all values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="131">
   <si>
     <t>As a hotel owner I want a payment details portal so that I can assist my customers</t>
   </si>
@@ -388,6 +433,129 @@
   </si>
   <si>
     <t>A00426488</t>
+  </si>
+  <si>
+    <t>As a customer I want to see my pervious bookings so that I can see what I paid ( compare prices)</t>
+  </si>
+  <si>
+    <t>As a customer I want to get an email notification of payment so that I can have proof of payment</t>
+  </si>
+  <si>
+    <t>As a hotel owner I want to see the resurant menu so that customers will know what food options there are</t>
+  </si>
+  <si>
+    <t>As a customer I want to have an option to book a meeting hall so that I can online book an event</t>
+  </si>
+  <si>
+    <t>As a hotel owner I want a special role so that I can have different access for different users ( admin/users)</t>
+  </si>
+  <si>
+    <t>As a hotel owner I want to implement a live chat for employees so that I can assist my customers in real time</t>
+  </si>
+  <si>
+    <t>As a customer I want to schedue an airport pickup so that I be picked up by the hotel airport shuttle</t>
+  </si>
+  <si>
+    <t>As a customer I want to re-schedue an airport pickup so that I be picked up by the hotel airport shuttle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Retrieve pickup schedule for customer by ID from Schedule Table</t>
+  </si>
+  <si>
+    <t>Set function to update details</t>
+  </si>
+  <si>
+    <t>Add portal in website for customer to input detail</t>
+  </si>
+  <si>
+    <t>Integrate portal with data base</t>
+  </si>
+  <si>
+    <t>Integration testin</t>
+  </si>
+  <si>
+    <t>Succesful update of existing schedule</t>
+  </si>
+  <si>
+    <t>Retreieve past payment details based on customer ID</t>
+  </si>
+  <si>
+    <t>Add section to payment portal in customer side of the website</t>
+  </si>
+  <si>
+    <t>Put into tabular format in website</t>
+  </si>
+  <si>
+    <t>Show generated report</t>
+  </si>
+  <si>
+    <t>Customer can view all past details</t>
+  </si>
+  <si>
+    <t>Get menu from restaurants in Hotel</t>
+  </si>
+  <si>
+    <t>Build portal in website</t>
+  </si>
+  <si>
+    <t>Update portal information</t>
+  </si>
+  <si>
+    <t>Add Menus database</t>
+  </si>
+  <si>
+    <t>Integrate database with website</t>
+  </si>
+  <si>
+    <t>Add menus to database</t>
+  </si>
+  <si>
+    <t>exit criteria</t>
+  </si>
+  <si>
+    <t>Restaurant menu uploaded on website</t>
+  </si>
+  <si>
+    <t>Restaurant menu viewable on website</t>
+  </si>
+  <si>
+    <t>Retreive information from Payment API Already created</t>
+  </si>
+  <si>
+    <t>Sort the payments according to date</t>
+  </si>
+  <si>
+    <t>Store the information on a particular date in tabular format</t>
+  </si>
+  <si>
+    <t>Build Payment API portal option with date selection</t>
+  </si>
+  <si>
+    <t>Connect API to the new functionaility</t>
+  </si>
+  <si>
+    <t>Provider can view the details on a date on website</t>
+  </si>
+  <si>
+    <t>As a payment provider I want Payment info in a database so that I can see all my data for reports </t>
+  </si>
+  <si>
+    <t>As a payment provider I want customer specific portal so that my customers can look at their transaction data directly </t>
+  </si>
+  <si>
+    <t>As a hotel customer I want a user portal so that I can cancel my booking </t>
+  </si>
+  <si>
+    <t>As a hotel customer I want a user portal so that I can edit my booking </t>
+  </si>
+  <si>
+    <t>As an owner I want to review/feedback page visible by owner so that I can improve customer satisfaction </t>
+  </si>
+  <si>
+    <t>As a payment provider  I want an Payment API available so that I can troubleshoot payment issues</t>
   </si>
 </sst>
 </file>
@@ -424,7 +592,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,6 +602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,11 +624,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,6 +697,50 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{076B6587-CEE2-3543-91D2-30B7D44799FD}" name="Tasks"/>
     <tableColumn id="2" xr3:uid="{C89922EB-30BD-D745-99B8-75201257D3B2}" name="Effort"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DAEAC8BA-6958-7449-8FA4-836C85E51CE8}" name="Table13457" displayName="Table13457" ref="A8:B23" totalsRowShown="0">
+  <autoFilter ref="A8:B23" xr:uid="{6BE16BF6-F9BF-5841-AB81-A6CF7E999667}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{01F4520A-6D17-1544-83AD-7A25E41E8173}" name="Tasks"/>
+    <tableColumn id="2" xr3:uid="{9BA2EF2A-B3E4-BA4E-B5FA-7C80A3D09A36}" name="Effort"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{484986D5-5AE2-FD49-BA50-0E74C3EFB354}" name="Table134578" displayName="Table134578" ref="A26:B41" totalsRowShown="0">
+  <autoFilter ref="A26:B41" xr:uid="{3B43298A-A34B-2149-93A0-AB0CE44F4A6A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{81A0160E-7697-7B4A-BB6C-C02E4491581D}" name="Tasks"/>
+    <tableColumn id="2" xr3:uid="{2F4AE5CF-3831-1B4F-94FF-CF2D13A0FFEE}" name="Effort"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{80DCC052-BEB4-B24F-A769-858DC28350D8}" name="Table1345789" displayName="Table1345789" ref="A44:B61" totalsRowShown="0">
+  <autoFilter ref="A44:B61" xr:uid="{75476F78-5D6E-0348-B4D5-B0724AFE7230}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E5B6E24A-1504-1E45-A477-15A521C377B6}" name="Tasks"/>
+    <tableColumn id="2" xr3:uid="{0D048A92-DBC3-A34D-8F45-02D9D7BE1038}" name="Effort"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0A7C1374-4D8D-1E47-9DC3-A2F3EBBD5F16}" name="Table134578910" displayName="Table134578910" ref="A64:B79" totalsRowShown="0">
+  <autoFilter ref="A64:B79" xr:uid="{B6BE7031-212E-834B-9A3E-4A92F6BB5B9E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{BDBF0568-6E1A-714D-BA74-5C206D93C6A4}" name="Tasks"/>
+    <tableColumn id="2" xr3:uid="{39CC65EB-9B3A-4543-A4C4-EDF677865CA8}" name="Effort"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -896,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="134" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A10" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="171" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,63 +1303,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>40</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>0.5</v>
       </c>
-      <c r="D2" s="2">
-        <f t="shared" ref="D2:D18" si="0">B2/C2</f>
+      <c r="D2">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3">
         <v>40</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <f t="shared" si="0"/>
+      <c r="D3">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>40</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>0.5</v>
       </c>
-      <c r="D5" s="2">
-        <f t="shared" si="0"/>
+      <c r="D5">
         <v>16</v>
       </c>
     </row>
@@ -1154,8 +1369,7 @@
       <c r="C6">
         <v>0.5</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
+      <c r="D6">
         <v>10</v>
       </c>
     </row>
@@ -1169,14 +1383,13 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
+      <c r="D7">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>126</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -1184,14 +1397,13 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
+      <c r="D8">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -1199,14 +1411,13 @@
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
+      <c r="D9">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="B10">
         <v>20</v>
@@ -1214,8 +1425,7 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
+      <c r="D10">
         <v>4</v>
       </c>
     </row>
@@ -1229,8 +1439,7 @@
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
+      <c r="D11">
         <v>2</v>
       </c>
     </row>
@@ -1244,14 +1453,13 @@
       <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
+      <c r="D12">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="B13">
         <v>40</v>
@@ -1259,8 +1467,7 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
+      <c r="D13">
         <v>2</v>
       </c>
     </row>
@@ -1274,8 +1481,7 @@
       <c r="C14">
         <v>20</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
+      <c r="D14">
         <v>1</v>
       </c>
     </row>
@@ -1289,8 +1495,7 @@
       <c r="C15">
         <v>40</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
+      <c r="D15">
         <v>1</v>
       </c>
     </row>
@@ -1304,14 +1509,13 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+      <c r="D16">
+        <v>0.66666667000000002</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -1319,8 +1523,7 @@
       <c r="C17">
         <v>20</v>
       </c>
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
+      <c r="D17">
         <v>0.4</v>
       </c>
     </row>
@@ -1334,14 +1537,37 @@
       <c r="C18">
         <v>20</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
+      <c r="D18">
         <v>0.25</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="1"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:D18">
-    <sortCondition descending="1" ref="D1"/>
+  <sortState ref="A2:D26">
+    <sortCondition descending="1" ref="D26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1352,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1443,6 +1669,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>18</v>
@@ -1480,36 +1711,57 @@
       <c r="E25" t="s">
         <v>75</v>
       </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
         <v>66</v>
       </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
         <v>78</v>
       </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>77</v>
       </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>80</v>
       </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
         <v>67</v>
       </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
         <v>61</v>
       </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E34" t="s">
@@ -1543,36 +1795,57 @@
       <c r="E44" t="s">
         <v>69</v>
       </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E45" t="s">
         <v>76</v>
       </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E46" t="s">
         <v>70</v>
       </c>
+      <c r="F46">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
         <v>71</v>
       </c>
+      <c r="F47">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E48" t="s">
         <v>72</v>
       </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E49" t="s">
         <v>67</v>
       </c>
+      <c r="F49">
+        <v>5</v>
+      </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
         <v>61</v>
       </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E52" t="s">
@@ -1601,38 +1874,56 @@
       <c r="E63" t="s">
         <v>81</v>
       </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E64" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E65" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E66" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E67" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E68" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E71" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E72" t="s">
         <v>84</v>
       </c>
@@ -1650,6 +1941,708 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D78D439-B5ED-9041-9424-113B4D239A20}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="100.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="1">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D26" si="0">B2/C2</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="4">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CAC81F-E7C5-EE4E-A85D-5C5F6DBF08E5}">
+  <dimension ref="A4:B72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="91.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>

</xml_diff>